<commit_message>
Adding a CLI interface
</commit_message>
<xml_diff>
--- a/worksheets/BookToValidate01.xlsx
+++ b/worksheets/BookToValidate01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/712e76bdfa434146/Documents/githubProjects/validator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/712e76bdfa434146/Documents/githubProjects/validator/worksheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{F28AEF14-B32A-41F3-B98D-9AD63FFECF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3954C54-57D0-4736-8194-F9DF0C68B1A1}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{F28AEF14-B32A-41F3-B98D-9AD63FFECF30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86428744-1F8C-45FE-BE28-E40540B147C6}"/>
   <bookViews>
-    <workbookView xWindow="34200" yWindow="2805" windowWidth="13305" windowHeight="11385" xr2:uid="{48B41AE7-338C-46D3-B278-C9ABE81569C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{48B41AE7-338C-46D3-B278-C9ABE81569C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Book_01" sheetId="1" r:id="rId1"/>
@@ -399,7 +399,7 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">

</xml_diff>